<commit_message>
update files with latest copies in def store develop branch
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/CCD_BEFTA_JURISDICTION2.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/CCD_BEFTA_JURISDICTION2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10112"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veeresha/hmcts/git/ccd-data-store-api/src/aat/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/475495/Documents/Home/Development/06-Jan/ccd-data-store/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F8D42F-787B-4646-8BB5-39AF2908318E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26AACA2-0136-034D-B20E-1BCD5F8E6D7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="17180" tabRatio="823" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="17180" tabRatio="823" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -26,18 +26,17 @@
     <sheet name="WorkBasketInputFields" sheetId="17" r:id="rId11"/>
     <sheet name="WorkBasketResultFields" sheetId="11" r:id="rId12"/>
     <sheet name="CaseTypeTab" sheetId="12" r:id="rId13"/>
-    <sheet name="CaseRoles" sheetId="20" r:id="rId14"/>
-    <sheet name="UserProfile" sheetId="16" r:id="rId15"/>
-    <sheet name="AuthorisationCaseType" sheetId="13" r:id="rId16"/>
-    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId17"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="15" r:id="rId18"/>
-    <sheet name="AuthorisationCaseField" sheetId="14" r:id="rId19"/>
-    <sheet name="AuthorisationComplexType" sheetId="19" r:id="rId20"/>
+    <sheet name="UserProfile" sheetId="16" r:id="rId14"/>
+    <sheet name="AuthorisationCaseType" sheetId="13" r:id="rId15"/>
+    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId16"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="15" r:id="rId17"/>
+    <sheet name="AuthorisationCaseField" sheetId="14" r:id="rId18"/>
+    <sheet name="AuthorisationComplexType" sheetId="19" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">AuthorisationCaseField!$A$1:$F$111</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">AuthorisationCaseField!$A$1:$F$111</definedName>
   </definedNames>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2645" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2629" uniqueCount="311">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -998,21 +997,6 @@
   </si>
   <si>
     <t>befta.caseworker.2.solicitor.3@gmail.com</t>
-  </si>
-  <si>
-    <t>CaseRoles</t>
-  </si>
-  <si>
-    <t>MaxLength:128</t>
-  </si>
-  <si>
-    <t>[DEFENDANT]</t>
-  </si>
-  <si>
-    <t>Defendant</t>
-  </si>
-  <si>
-    <t>The defending party</t>
   </si>
 </sst>
 </file>
@@ -1024,7 +1008,7 @@
     <numFmt numFmtId="165" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="44" x14ac:knownFonts="1">
+  <fonts count="42" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1303,18 +1287,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF632523"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1348,7 +1320,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1401,43 +1373,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1470,7 +1405,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1593,16 +1528,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="42" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -3656,83 +3581,6 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB450B91-5B56-6749-90B2-76213C388519}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="88" t="s">
-        <v>311</v>
-      </c>
-      <c r="B1" s="89" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="90" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="91" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="92" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="93" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="93" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="93" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="94" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="95" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="96" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="96" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="28" t="s">
-        <v>271</v>
-      </c>
-      <c r="B4" s="97" t="s">
-        <v>313</v>
-      </c>
-      <c r="C4" s="97" t="s">
-        <v>314</v>
-      </c>
-      <c r="D4" s="97" t="s">
-        <v>315</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -3891,7 +3739,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -4054,7 +3902,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
@@ -4460,7 +4308,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
@@ -5194,13 +5042,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView topLeftCell="C83" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="F119" sqref="F119:F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7427,6 +7275,351 @@
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="144" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="80" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="80" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="80" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.6640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.6640625" style="80" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="80" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="80"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="75" t="s">
+        <v>261</v>
+      </c>
+      <c r="B1" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="78" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+    </row>
+    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
+      <c r="A2" s="81"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="82" t="s">
+        <v>262</v>
+      </c>
+      <c r="D2" s="82" t="s">
+        <v>263</v>
+      </c>
+      <c r="E2" s="82" t="s">
+        <v>264</v>
+      </c>
+      <c r="F2" s="82" t="s">
+        <v>265</v>
+      </c>
+      <c r="G2" s="82" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="83" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="83" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="84" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="84" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="84" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="85" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" s="85" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="G4" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="G5" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="G6" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="G7" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="G8" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E9" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="G9" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="G10" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="G11" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="G12" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="G13" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="G14" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="G15" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="71"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="71"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="71"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -7585,356 +7778,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
-  <dimension ref="A1:G18"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="144" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="33.1640625" style="80" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="80" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="80" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="80" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.6640625" style="80" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.6640625" style="80" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="80" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="80"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="75" t="s">
-        <v>261</v>
-      </c>
-      <c r="B1" s="76" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="77" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="78" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-    </row>
-    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
-      <c r="A2" s="81"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="82" t="s">
-        <v>262</v>
-      </c>
-      <c r="D2" s="82" t="s">
-        <v>263</v>
-      </c>
-      <c r="E2" s="82" t="s">
-        <v>264</v>
-      </c>
-      <c r="F2" s="82" t="s">
-        <v>265</v>
-      </c>
-      <c r="G2" s="82" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="83" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="83" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="84" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="84" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="84" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="85" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" s="85" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D4" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>213</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="G4" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D5" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E5" s="41" t="s">
-        <v>215</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="G5" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D6" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E6" s="41" t="s">
-        <v>221</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="G6" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D7" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E7" s="41" t="s">
-        <v>213</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>305</v>
-      </c>
-      <c r="G7" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D8" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E8" s="41" t="s">
-        <v>215</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>305</v>
-      </c>
-      <c r="G8" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D9" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E9" s="41" t="s">
-        <v>221</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>305</v>
-      </c>
-      <c r="G9" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D10" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E10" s="41" t="s">
-        <v>213</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>306</v>
-      </c>
-      <c r="G10" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D11" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E11" s="41" t="s">
-        <v>215</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>306</v>
-      </c>
-      <c r="G11" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D12" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E12" s="41" t="s">
-        <v>221</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>306</v>
-      </c>
-      <c r="G12" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D13" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E13" s="41" t="s">
-        <v>213</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>309</v>
-      </c>
-      <c r="G13" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D14" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E14" s="41" t="s">
-        <v>215</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>309</v>
-      </c>
-      <c r="G14" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D15" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E15" s="41" t="s">
-        <v>221</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>309</v>
-      </c>
-      <c r="G15" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="71"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A17" s="71"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="14"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18" s="71"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="14"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="D4" sqref="D4:D26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update version with case role DEFENDANT
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/CCD_BEFTA_JURISDICTION2.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/CCD_BEFTA_JURISDICTION2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/475495/Documents/Home/Development/06-Jan/ccd-data-store/src/aat/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veeresha/hmcts/git/ccd-data-store-api/src/aat/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26AACA2-0136-034D-B20E-1BCD5F8E6D7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F8D42F-787B-4646-8BB5-39AF2908318E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="17180" tabRatio="823" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="17180" tabRatio="823" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -26,17 +26,18 @@
     <sheet name="WorkBasketInputFields" sheetId="17" r:id="rId11"/>
     <sheet name="WorkBasketResultFields" sheetId="11" r:id="rId12"/>
     <sheet name="CaseTypeTab" sheetId="12" r:id="rId13"/>
-    <sheet name="UserProfile" sheetId="16" r:id="rId14"/>
-    <sheet name="AuthorisationCaseType" sheetId="13" r:id="rId15"/>
-    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId16"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="15" r:id="rId17"/>
-    <sheet name="AuthorisationCaseField" sheetId="14" r:id="rId18"/>
-    <sheet name="AuthorisationComplexType" sheetId="19" r:id="rId19"/>
+    <sheet name="CaseRoles" sheetId="20" r:id="rId14"/>
+    <sheet name="UserProfile" sheetId="16" r:id="rId15"/>
+    <sheet name="AuthorisationCaseType" sheetId="13" r:id="rId16"/>
+    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId17"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="15" r:id="rId18"/>
+    <sheet name="AuthorisationCaseField" sheetId="14" r:id="rId19"/>
+    <sheet name="AuthorisationComplexType" sheetId="19" r:id="rId20"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">AuthorisationCaseField!$A$1:$F$111</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">AuthorisationCaseField!$A$1:$F$111</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2629" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2645" uniqueCount="316">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -997,6 +998,21 @@
   </si>
   <si>
     <t>befta.caseworker.2.solicitor.3@gmail.com</t>
+  </si>
+  <si>
+    <t>CaseRoles</t>
+  </si>
+  <si>
+    <t>MaxLength:128</t>
+  </si>
+  <si>
+    <t>[DEFENDANT]</t>
+  </si>
+  <si>
+    <t>Defendant</t>
+  </si>
+  <si>
+    <t>The defending party</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1024,7 @@
     <numFmt numFmtId="165" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="42" x14ac:knownFonts="1">
+  <fonts count="44" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1287,6 +1303,18 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF632523"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1320,7 +1348,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1373,6 +1401,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1405,7 +1470,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1528,6 +1593,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="42" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -3581,6 +3656,83 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB450B91-5B56-6749-90B2-76213C388519}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="88" t="s">
+        <v>311</v>
+      </c>
+      <c r="B1" s="89" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="90" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="91" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" s="92" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="93" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="93" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="93" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="94" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="96" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="96" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" s="28" t="s">
+        <v>271</v>
+      </c>
+      <c r="B4" s="97" t="s">
+        <v>313</v>
+      </c>
+      <c r="C4" s="97" t="s">
+        <v>314</v>
+      </c>
+      <c r="D4" s="97" t="s">
+        <v>315</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -3739,7 +3891,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -3902,7 +4054,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
@@ -4308,7 +4460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
@@ -5042,13 +5194,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="F119" sqref="F119:F125"/>
+    <sheetView topLeftCell="C83" workbookViewId="0">
+      <selection activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7275,351 +7427,6 @@
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
-  <dimension ref="A1:G18"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="144" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="33.1640625" style="80" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="80" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="80" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="80" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.6640625" style="80" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.6640625" style="80" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="80" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="80"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="75" t="s">
-        <v>261</v>
-      </c>
-      <c r="B1" s="76" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="77" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="78" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-    </row>
-    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
-      <c r="A2" s="81"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="82" t="s">
-        <v>262</v>
-      </c>
-      <c r="D2" s="82" t="s">
-        <v>263</v>
-      </c>
-      <c r="E2" s="82" t="s">
-        <v>264</v>
-      </c>
-      <c r="F2" s="82" t="s">
-        <v>265</v>
-      </c>
-      <c r="G2" s="82" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="83" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="83" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="84" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="84" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="84" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="85" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" s="85" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D4" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>213</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="G4" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D5" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E5" s="41" t="s">
-        <v>215</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="G5" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D6" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E6" s="41" t="s">
-        <v>221</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="G6" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D7" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E7" s="41" t="s">
-        <v>213</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>305</v>
-      </c>
-      <c r="G7" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D8" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E8" s="41" t="s">
-        <v>215</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>305</v>
-      </c>
-      <c r="G8" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D9" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E9" s="41" t="s">
-        <v>221</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>305</v>
-      </c>
-      <c r="G9" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D10" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E10" s="41" t="s">
-        <v>213</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>306</v>
-      </c>
-      <c r="G10" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D11" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E11" s="41" t="s">
-        <v>215</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>306</v>
-      </c>
-      <c r="G11" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D12" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E12" s="41" t="s">
-        <v>221</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>306</v>
-      </c>
-      <c r="G12" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D13" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E13" s="41" t="s">
-        <v>213</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>309</v>
-      </c>
-      <c r="G13" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D14" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E14" s="41" t="s">
-        <v>215</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>309</v>
-      </c>
-      <c r="G14" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="71">
-        <v>42736</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="D15" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="E15" s="41" t="s">
-        <v>221</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>309</v>
-      </c>
-      <c r="G15" s="80" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="71"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A17" s="71"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="14"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18" s="71"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="14"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -7778,11 +7585,356 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBCB2E-F376-5E45-8D3D-BA39DB091F6A}">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="144" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="80" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="80" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="80" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.6640625" style="80" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.6640625" style="80" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="80" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="80"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="75" t="s">
+        <v>261</v>
+      </c>
+      <c r="B1" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="78" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+    </row>
+    <row r="2" spans="1:7" ht="70" x14ac:dyDescent="0.15">
+      <c r="A2" s="81"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="82" t="s">
+        <v>262</v>
+      </c>
+      <c r="D2" s="82" t="s">
+        <v>263</v>
+      </c>
+      <c r="E2" s="82" t="s">
+        <v>264</v>
+      </c>
+      <c r="F2" s="82" t="s">
+        <v>265</v>
+      </c>
+      <c r="G2" s="82" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="83" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="83" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="84" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="84" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="84" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="85" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" s="85" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="G4" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="G5" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="G6" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="G7" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="G8" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E9" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="G9" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="G10" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="G11" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="G12" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="G13" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="G14" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="71">
+        <v>42736</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="G15" s="80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="71"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="71"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="71"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="D4" sqref="D4:D26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
synch file with data store develop
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/CCD_BEFTA_JURISDICTION2.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/CCD_BEFTA_JURISDICTION2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veeresha/hmcts/git/ccd-data-store-api/src/aat/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/HMCTS/DEVLAB/WS/STS_HMCTS/CCD/ccd-api-test-automation-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F8D42F-787B-4646-8BB5-39AF2908318E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E925211B-349D-9E4A-883D-4347989BC5BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="17180" tabRatio="823" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3660,7 +3660,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>